<commit_message>
formatacao cond por formulas
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/5.Formatacao/4.Formatacao_condicional_formulas.xlsx
+++ b/2.Excel/hands-on/5.Formatacao/4.Formatacao_condicional_formulas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55219\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\5.Formatacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911C0854-87F3-4DC0-88F8-15C12CB36AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484240FD-7E1E-4420-87B6-8BD48FAAFC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{42A226BC-69FF-4E1F-AF6F-5464E52F4861}"/>
+    <workbookView xWindow="11280" yWindow="0" windowWidth="11868" windowHeight="12792" xr2:uid="{42A226BC-69FF-4E1F-AF6F-5464E52F4861}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,7 +141,20 @@
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -155,7 +168,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -453,17 +466,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58FACA41-9270-4015-9A56-C1FA05D94F28}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.899999999999999">
+    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -475,7 +488,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="16.899999999999999">
+    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -483,10 +496,14 @@
         <v>1426</v>
       </c>
       <c r="C2" s="2">
-        <v>45112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16.899999999999999">
+        <v>45296</v>
+      </c>
+      <c r="E2" t="b">
+        <f ca="1">C2&lt;TODAY()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -494,10 +511,14 @@
         <v>1472</v>
       </c>
       <c r="C3" s="2">
-        <v>45109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16.899999999999999">
+        <v>45475</v>
+      </c>
+      <c r="E3" t="b">
+        <f t="shared" ref="E3:E10" ca="1" si="0">C3&lt;TODAY()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -505,10 +526,14 @@
         <v>1433</v>
       </c>
       <c r="C4" s="2">
-        <v>45105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="16.899999999999999">
+        <v>45471</v>
+      </c>
+      <c r="E4" t="b">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -518,8 +543,12 @@
       <c r="C5" s="2">
         <v>45117</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.899999999999999">
+      <c r="E5" t="b">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -529,8 +558,12 @@
       <c r="C6" s="2">
         <v>45148</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.899999999999999">
+      <c r="E6" t="b">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -538,10 +571,14 @@
         <v>1308</v>
       </c>
       <c r="C7" s="2">
-        <v>45140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.899999999999999">
+        <v>45506</v>
+      </c>
+      <c r="E7" t="b">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -551,8 +588,12 @@
       <c r="C8" s="2">
         <v>45111</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="16.899999999999999">
+      <c r="E8" t="b">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -560,10 +601,14 @@
         <v>1999</v>
       </c>
       <c r="C9" s="2">
-        <v>45105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16.899999999999999">
+        <v>45319</v>
+      </c>
+      <c r="E9" t="b">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -571,10 +616,19 @@
         <v>1477</v>
       </c>
       <c r="C10" s="2">
-        <v>45164</v>
+        <v>45293</v>
+      </c>
+      <c r="E10" t="b">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>C2&lt;TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>